<commit_message>
Omstrukturert pakke - skilt ut variabeldefinisjon, men ikke figur. Fungerer for valgtVar='Alder'
</commit_message>
<xml_diff>
--- a/doc/NorSpis Bestillingsskjema nye figurer 16 08 16.xlsx
+++ b/doc/NorSpis Bestillingsskjema nye figurer 16 08 16.xlsx
@@ -14,6 +14,9 @@
   <externalReferences>
     <externalReference r:id="rId4"/>
   </externalReferences>
+  <definedNames>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">Bestilling!$20:$20</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
@@ -315,9 +318,6 @@
     <t>EDQ delskårer, flere figurer</t>
   </si>
   <si>
-    <t>Oppdatert: 03.05.2016</t>
-  </si>
-  <si>
     <t>I neste runde må vi huske å ta med resultater for Tiltak og Behandlingstilnærming</t>
   </si>
   <si>
@@ -715,10 +715,6 @@
     <t>CIA30GlobalScore</t>
   </si>
   <si>
-    <t>Intervaller: &lt;11, 11-13, 14-15, 16-17, 18-19, 20-24, 25-29, 30-39, 40-49, 50-59, 60+
-(Har nå brukt 5-åringe intervaller)</t>
-  </si>
-  <si>
     <t>ok</t>
   </si>
   <si>
@@ -729,6 +725,26 @@
   </si>
   <si>
     <t>Høyeste fullførte utdanning</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Intervaller: &lt;11, 11-13, 14-15, 16-17, 18-19, 20-24, 25-29, 30-39, 40-49, 50-59, 60+
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Har nå brukt 5-åringe intervaller)</t>
+    </r>
+  </si>
+  <si>
+    <t>Oppdatert: aug.2016</t>
   </si>
 </sst>
 </file>
@@ -1662,9 +1678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="20" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A21" sqref="A21:XFD21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -1685,7 +1700,7 @@
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" ht="15.75">
       <c r="A2" s="9" t="s">
-        <v>91</v>
+        <v>208</v>
       </c>
       <c r="B2" s="9"/>
       <c r="D2" s="12"/>
@@ -1877,7 +1892,7 @@
     <row r="21" spans="1:7" s="7" customFormat="1" ht="18.75">
       <c r="A21" s="6"/>
       <c r="B21" s="31" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="14"/>
@@ -1892,7 +1907,7 @@
         <v>2</v>
       </c>
       <c r="B23" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C23" s="24" t="s">
         <v>4</v>
@@ -1901,10 +1916,10 @@
         <v>0</v>
       </c>
       <c r="E23" s="32" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F23" s="25" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="G23" s="25"/>
     </row>
@@ -1916,10 +1931,10 @@
         <v>34</v>
       </c>
       <c r="D24" s="24" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E24" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F24" s="24" t="s">
         <v>35</v>
@@ -1933,13 +1948,13 @@
         <v>34</v>
       </c>
       <c r="D25" s="24" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F25" s="24" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="30">
@@ -1950,10 +1965,10 @@
         <v>30</v>
       </c>
       <c r="D26" s="25" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E26" s="25" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1964,7 +1979,7 @@
         <v>38</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F27" t="s">
         <v>39</v>
@@ -1975,7 +1990,7 @@
         <v>2</v>
       </c>
       <c r="B28" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C28" s="24" t="s">
         <v>40</v>
@@ -1984,7 +1999,7 @@
         <v>40</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1996,10 +2011,10 @@
       </c>
       <c r="D29" s="15"/>
       <c r="E29" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F29" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -2007,10 +2022,10 @@
         <v>64</v>
       </c>
       <c r="D30" s="15" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E30" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="45">
@@ -2021,13 +2036,13 @@
         <v>42</v>
       </c>
       <c r="D31" s="34" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E31" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F31" s="32" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -2038,10 +2053,10 @@
         <v>43</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="30">
@@ -2052,10 +2067,10 @@
         <v>55</v>
       </c>
       <c r="D33" s="15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E33" s="24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="30">
@@ -2066,10 +2081,10 @@
         <v>45</v>
       </c>
       <c r="D34" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E34" s="24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="30">
@@ -2077,16 +2092,16 @@
         <v>2</v>
       </c>
       <c r="B35" t="s">
+        <v>203</v>
+      </c>
+      <c r="C35" s="24" t="s">
         <v>205</v>
       </c>
-      <c r="C35" s="24" t="s">
-        <v>207</v>
-      </c>
       <c r="D35" s="15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E35" s="24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="30">
@@ -2094,13 +2109,13 @@
         <v>2</v>
       </c>
       <c r="C36" s="24" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D36" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E36" s="24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="30">
@@ -2108,13 +2123,13 @@
         <v>2</v>
       </c>
       <c r="C37" s="24" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D37" s="15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E37" s="24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="30">
@@ -2125,10 +2140,10 @@
         <v>56</v>
       </c>
       <c r="D38" s="15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E38" s="24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="45">
@@ -2139,10 +2154,10 @@
         <v>57</v>
       </c>
       <c r="D39" s="15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E39" s="24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="45">
@@ -2153,10 +2168,10 @@
         <v>58</v>
       </c>
       <c r="D40" s="15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E40" s="24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="45">
@@ -2167,10 +2182,10 @@
         <v>59</v>
       </c>
       <c r="D41" s="15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E41" s="24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>60</v>
@@ -2181,16 +2196,16 @@
         <v>2</v>
       </c>
       <c r="C42" s="24" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D42" s="15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E42" s="24" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F42" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="30">
@@ -2198,13 +2213,13 @@
         <v>2</v>
       </c>
       <c r="C43" s="24" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D43" s="33" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E43" s="24" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>61</v>
@@ -2218,10 +2233,10 @@
         <v>62</v>
       </c>
       <c r="D44" s="33" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E44" s="24" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>63</v>
@@ -2232,13 +2247,13 @@
         <v>2</v>
       </c>
       <c r="C45" s="24" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D45" s="34" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E45" s="24" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="120">
@@ -2249,13 +2264,13 @@
         <v>65</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E46" s="24" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F46" s="24" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="45">
@@ -2266,13 +2281,13 @@
         <v>46</v>
       </c>
       <c r="D47" s="25" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E47" s="24" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F47" s="24" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="45">
@@ -2283,10 +2298,10 @@
         <v>46</v>
       </c>
       <c r="D48" s="25" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E48" s="24" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F48" t="s">
         <v>66</v>
@@ -2300,10 +2315,10 @@
         <v>46</v>
       </c>
       <c r="D49" s="25" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E49" s="24" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F49" t="s">
         <v>67</v>
@@ -2314,13 +2329,13 @@
         <v>2</v>
       </c>
       <c r="C50" s="24" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D50" s="25" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E50" s="24" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F50" t="s">
         <v>68</v>
@@ -2331,13 +2346,13 @@
         <v>2</v>
       </c>
       <c r="C51" s="24" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D51" s="25" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E51" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>70</v>
@@ -2348,13 +2363,13 @@
         <v>2</v>
       </c>
       <c r="C52" s="24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E52" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>71</v>
@@ -2368,13 +2383,13 @@
         <v>72</v>
       </c>
       <c r="D53" s="25" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E53" s="24" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="60">
@@ -2385,10 +2400,10 @@
         <v>74</v>
       </c>
       <c r="D54" s="25" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E54" s="24" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F54" s="1" t="s">
         <v>73</v>
@@ -2399,13 +2414,13 @@
         <v>2</v>
       </c>
       <c r="C55" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E55" s="24" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="30">
@@ -2416,10 +2431,10 @@
         <v>75</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E56" s="24" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -2427,13 +2442,13 @@
         <v>2</v>
       </c>
       <c r="C57" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D57" s="25" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E57" s="24" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -2441,13 +2456,13 @@
         <v>2</v>
       </c>
       <c r="C58" s="24" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D58" s="25" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E58" s="24" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="180">
@@ -2455,13 +2470,13 @@
         <v>2</v>
       </c>
       <c r="C59" s="24" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D59" s="25" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E59" s="24" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F59" t="s">
         <v>76</v>
@@ -2472,16 +2487,16 @@
         <v>2</v>
       </c>
       <c r="C60" s="24" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D60" s="25" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E60" s="24" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -2489,13 +2504,13 @@
         <v>24</v>
       </c>
       <c r="C63" s="24" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>77</v>
       </c>
       <c r="E63" s="24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="60">
@@ -2503,16 +2518,16 @@
         <v>24</v>
       </c>
       <c r="C64" s="24" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D64" s="35" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E64" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F64" s="24" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="65" spans="1:11" ht="75">
@@ -2520,13 +2535,13 @@
         <v>24</v>
       </c>
       <c r="C65" s="24" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D65" s="36" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E65" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F65" t="s">
         <v>84</v>
@@ -2540,10 +2555,10 @@
         <v>46</v>
       </c>
       <c r="D66" s="36" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E66" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F66" t="s">
         <v>84</v>
@@ -2554,10 +2569,10 @@
         <v>24</v>
       </c>
       <c r="D67" s="25" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E67" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F67" t="s">
         <v>85</v>
@@ -2571,13 +2586,13 @@
         <v>24</v>
       </c>
       <c r="C68" s="24" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D68" s="25" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E68" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F68" t="s">
         <v>78</v>
@@ -2592,13 +2607,13 @@
         <v>24</v>
       </c>
       <c r="C69" s="24" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E69" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F69" t="s">
         <v>79</v>
@@ -2614,13 +2629,13 @@
         <v>24</v>
       </c>
       <c r="C70" s="24" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E70" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F70" t="s">
         <v>80</v>
@@ -2631,13 +2646,13 @@
         <v>24</v>
       </c>
       <c r="C71" s="24" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E71" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F71" t="s">
         <v>81</v>
@@ -2651,10 +2666,10 @@
         <v>69</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E72" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F72" t="s">
         <v>82</v>
@@ -2668,13 +2683,13 @@
         <v>83</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E73" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F73" s="24" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="74" spans="1:11" ht="45">
@@ -2685,13 +2700,13 @@
         <v>31</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E74" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F74" s="24" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="75" spans="1:11" ht="45">
@@ -2702,10 +2717,10 @@
         <v>46</v>
       </c>
       <c r="E75" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F75" s="24" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="76" spans="1:11">
@@ -2713,13 +2728,13 @@
         <v>24</v>
       </c>
       <c r="C76" s="24" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E76" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="77" spans="1:11">
@@ -2727,13 +2742,13 @@
         <v>24</v>
       </c>
       <c r="C77" s="24" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F77" s="1" t="s">
         <v>86</v>
@@ -2744,13 +2759,13 @@
         <v>25</v>
       </c>
       <c r="C80" s="24" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D80" s="35" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E80" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F80" t="s">
         <v>87</v>
@@ -2761,13 +2776,13 @@
         <v>25</v>
       </c>
       <c r="C81" s="24" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E81" s="25" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="82" spans="1:9" ht="45">
@@ -2778,10 +2793,10 @@
         <v>88</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E82" s="25" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="83" spans="1:9">
@@ -2789,13 +2804,13 @@
         <v>25</v>
       </c>
       <c r="C83" s="24" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E83" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="84" spans="1:9" ht="135">
@@ -2803,13 +2818,13 @@
         <v>25</v>
       </c>
       <c r="C84" s="24" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D84" s="25" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E84" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F84" t="s">
         <v>89</v>
@@ -2817,24 +2832,24 @@
     </row>
     <row r="85" spans="1:9">
       <c r="C85" s="24" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E85" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="86" spans="1:9" ht="60">
       <c r="C86" s="24" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D86" s="25" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E86" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F86" t="s">
         <v>90</v>
@@ -2842,16 +2857,16 @@
     </row>
     <row r="87" spans="1:9" ht="135">
       <c r="C87" s="24" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D87" s="25" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E87" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F87" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="89" spans="1:9">
@@ -2873,7 +2888,7 @@
       <formula1>$A$8:$A$19</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="8" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
   <extLst>
@@ -3145,65 +3160,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100FCE962DAA607C141BEC58BE2E05A96D6" ma:contentTypeVersion="1" ma:contentTypeDescription="Opprett et nytt dokument." ma:contentTypeScope="" ma:versionID="7cda4e5099ab41e71e8155a34672a5e3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a191457c-5de3-4f0e-a27d-9676becc5466" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bfa2ff4172d93f67fbf5618108c0e081" ns2:_="">
     <xsd:import namespace="a191457c-5de3-4f0e-a27d-9676becc5466"/>
@@ -3348,33 +3304,82 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{407DBC2E-303A-497A-8115-DC0FA71100FD}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="a191457c-5de3-4f0e-a27d-9676becc5466"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0B1D3293-A2BB-4D4C-9BEF-6153B72ADE61}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77C70813-E504-4032-B3DB-29190042FFE1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00D81BE1-3A26-4FE1-92A1-915A7D7E5303}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3390,4 +3395,20 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77C70813-E504-4032-B3DB-29190042FFE1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0B1D3293-A2BB-4D4C-9BEF-6153B72ADE61}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>